<commit_message>
update add coop matrix for LPPI
</commit_message>
<xml_diff>
--- a/db/uploads/rate_new.xlsx
+++ b/db/uploads/rate_new.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>minAge</t>
   </si>
@@ -49,13 +49,26 @@
   <si>
     <t>Annual Premium Rate for ADB</t>
   </si>
+  <si>
+    <t>min coverage</t>
+  </si>
+  <si>
+    <t>max coverage</t>
+  </si>
+  <si>
+    <t>max Monthly Premium Rate</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -89,7 +102,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -227,53 +240,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -297,11 +269,9 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -583,668 +553,770 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>18</v>
       </c>
       <c r="B2" s="6">
         <v>65</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E2" s="7">
         <v>5</v>
       </c>
-      <c r="D2" s="8">
+      <c r="F2" s="8">
         <v>5.99</v>
       </c>
-      <c r="E2" s="8">
-        <f>C2/12</f>
+      <c r="G2" s="16">
+        <f>E2/12</f>
         <v>0.41666666666666669</v>
       </c>
-      <c r="F2" s="8">
-        <f>D2/12</f>
+      <c r="H2" s="16">
+        <f>F2/12</f>
         <v>0.4991666666666667</v>
       </c>
-      <c r="G2" s="8">
+      <c r="I2" s="8">
         <v>2.5</v>
       </c>
-      <c r="H2" s="8">
+      <c r="J2" s="8">
         <v>0.75</v>
       </c>
-      <c r="I2" s="8">
+      <c r="K2" s="8">
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>18</v>
       </c>
       <c r="B3" s="10">
         <v>65</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E3" s="11">
         <v>6</v>
       </c>
-      <c r="D3" s="12">
+      <c r="F3" s="12">
         <v>6.99</v>
       </c>
-      <c r="E3" s="12">
-        <f t="shared" ref="E3:F21" si="0">C3/12</f>
+      <c r="G3" s="17">
+        <f t="shared" ref="G3:G20" si="0">E3/12</f>
         <v>0.5</v>
       </c>
-      <c r="F3" s="12">
-        <f t="shared" si="0"/>
+      <c r="H3" s="17">
+        <f t="shared" ref="H3:H20" si="1">F3/12</f>
         <v>0.58250000000000002</v>
       </c>
-      <c r="G3" s="12">
+      <c r="I3" s="12">
         <v>7.5</v>
       </c>
-      <c r="H3" s="12">
+      <c r="J3" s="12">
         <v>0.81</v>
       </c>
-      <c r="I3" s="12">
+      <c r="K3" s="12">
         <v>0.61</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>18</v>
       </c>
       <c r="B4" s="10">
         <v>65</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="8">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E4" s="11">
         <v>7</v>
       </c>
-      <c r="D4" s="12">
+      <c r="F4" s="12">
         <v>7.99</v>
       </c>
-      <c r="E4" s="12">
+      <c r="G4" s="17">
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="F4" s="12">
-        <f t="shared" si="0"/>
+      <c r="H4" s="17">
+        <f t="shared" si="1"/>
         <v>0.66583333333333339</v>
       </c>
-      <c r="G4" s="12">
+      <c r="I4" s="12">
         <v>12.5</v>
       </c>
-      <c r="H4" s="12">
+      <c r="J4" s="12">
         <v>0.89</v>
       </c>
-      <c r="I4" s="12">
+      <c r="K4" s="12">
         <v>0.66</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>18</v>
       </c>
       <c r="B5" s="10">
         <v>65</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E5" s="11">
         <v>8</v>
       </c>
-      <c r="D5" s="12">
+      <c r="F5" s="12">
         <v>8.99</v>
       </c>
-      <c r="E5" s="12">
+      <c r="G5" s="17">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="F5" s="12">
-        <f t="shared" si="0"/>
+      <c r="H5" s="17">
+        <f t="shared" si="1"/>
         <v>0.74916666666666665</v>
       </c>
-      <c r="G5" s="12">
+      <c r="I5" s="12">
         <v>16.5</v>
       </c>
-      <c r="H5" s="12">
+      <c r="J5" s="12">
         <v>0.96</v>
       </c>
-      <c r="I5" s="12">
+      <c r="K5" s="12">
         <v>0.71</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>18</v>
       </c>
       <c r="B6" s="10">
         <v>65</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E6" s="11">
         <v>9</v>
       </c>
-      <c r="D6" s="12">
+      <c r="F6" s="12">
         <v>9.99</v>
       </c>
-      <c r="E6" s="12">
+      <c r="G6" s="17">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="F6" s="12">
-        <f t="shared" si="0"/>
+      <c r="H6" s="17">
+        <f t="shared" si="1"/>
         <v>0.83250000000000002</v>
       </c>
-      <c r="G6" s="12">
+      <c r="I6" s="12">
         <v>20.5</v>
       </c>
-      <c r="H6" s="12">
+      <c r="J6" s="12">
         <v>1.04</v>
       </c>
-      <c r="I6" s="13">
+      <c r="K6" s="13">
         <v>0.78</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>18</v>
       </c>
       <c r="B7" s="10">
         <v>65</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E7" s="11">
         <v>10</v>
       </c>
-      <c r="D7" s="12">
+      <c r="F7" s="12">
         <v>10.99</v>
       </c>
-      <c r="E7" s="12">
+      <c r="G7" s="17">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="F7" s="12">
-        <f t="shared" si="0"/>
+      <c r="H7" s="17">
+        <f t="shared" si="1"/>
         <v>0.91583333333333339</v>
       </c>
-      <c r="G7" s="12">
+      <c r="I7" s="12">
         <v>24.5</v>
       </c>
-      <c r="H7" s="12">
+      <c r="J7" s="12">
         <v>1.1299999999999999</v>
       </c>
-      <c r="I7" s="12">
+      <c r="K7" s="12">
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>18</v>
       </c>
       <c r="B8" s="10">
         <v>65</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E8" s="11">
         <v>11</v>
       </c>
-      <c r="D8" s="12">
+      <c r="F8" s="12">
         <v>11.99</v>
       </c>
-      <c r="E8" s="12">
+      <c r="G8" s="17">
         <f t="shared" si="0"/>
         <v>0.91666666666666663</v>
       </c>
-      <c r="F8" s="12">
-        <f t="shared" si="0"/>
+      <c r="H8" s="17">
+        <f t="shared" si="1"/>
         <v>0.99916666666666665</v>
       </c>
-      <c r="G8" s="12">
+      <c r="I8" s="12">
         <v>28.5</v>
       </c>
-      <c r="H8" s="12">
+      <c r="J8" s="12">
         <v>1.25</v>
       </c>
-      <c r="I8" s="12">
+      <c r="K8" s="12">
         <v>0.94</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>18</v>
       </c>
       <c r="B9" s="10">
         <v>65</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E9" s="11">
         <v>12</v>
       </c>
-      <c r="D9" s="12">
+      <c r="F9" s="12">
         <v>12.99</v>
       </c>
-      <c r="E9" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F9" s="12">
-        <f t="shared" si="0"/>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="17">
+        <f t="shared" si="1"/>
         <v>1.0825</v>
       </c>
-      <c r="G9" s="12">
+      <c r="I9" s="12">
         <v>32.5</v>
       </c>
-      <c r="H9" s="12">
+      <c r="J9" s="12">
         <v>1.39</v>
       </c>
-      <c r="I9" s="12">
+      <c r="K9" s="12">
         <v>1.05</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>18</v>
       </c>
       <c r="B10" s="10">
         <v>65</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="8">
+        <v>1</v>
+      </c>
+      <c r="D10" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E10" s="11">
         <v>13</v>
       </c>
-      <c r="D10" s="12">
+      <c r="F10" s="12">
         <v>13.99</v>
       </c>
-      <c r="E10" s="12">
+      <c r="G10" s="17">
         <f t="shared" si="0"/>
         <v>1.0833333333333333</v>
       </c>
-      <c r="F10" s="12">
-        <f t="shared" si="0"/>
+      <c r="H10" s="17">
+        <f t="shared" si="1"/>
         <v>1.1658333333333333</v>
       </c>
-      <c r="G10" s="12">
+      <c r="I10" s="12">
         <v>36.5</v>
       </c>
-      <c r="H10" s="12">
+      <c r="J10" s="12">
         <v>1.58</v>
       </c>
-      <c r="I10" s="12">
+      <c r="K10" s="12">
         <v>1.18</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>18</v>
       </c>
       <c r="B11" s="10">
         <v>65</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
+        <v>1</v>
+      </c>
+      <c r="D11" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E11" s="11">
         <v>14</v>
       </c>
-      <c r="D11" s="12">
+      <c r="F11" s="12">
         <v>14.99</v>
       </c>
-      <c r="E11" s="12">
+      <c r="G11" s="17">
         <f t="shared" si="0"/>
         <v>1.1666666666666667</v>
       </c>
-      <c r="F11" s="12">
-        <f t="shared" si="0"/>
+      <c r="H11" s="17">
+        <f t="shared" si="1"/>
         <v>1.2491666666666668</v>
       </c>
-      <c r="G11" s="12">
+      <c r="I11" s="12">
         <v>40.5</v>
       </c>
-      <c r="H11" s="12">
+      <c r="J11" s="12">
         <v>1.81</v>
       </c>
-      <c r="I11" s="12">
+      <c r="K11" s="12">
         <v>1.36</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>18</v>
       </c>
       <c r="B12" s="10">
         <v>65</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="8">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E12" s="11">
         <v>15</v>
       </c>
-      <c r="D12" s="12">
+      <c r="F12" s="12">
         <v>15.99</v>
       </c>
-      <c r="E12" s="12">
+      <c r="G12" s="17">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="F12" s="12">
-        <f t="shared" si="0"/>
+      <c r="H12" s="17">
+        <f t="shared" si="1"/>
         <v>1.3325</v>
       </c>
-      <c r="G12" s="12">
+      <c r="I12" s="12">
         <v>42.5</v>
       </c>
-      <c r="H12" s="12">
+      <c r="J12" s="12">
         <v>1.95</v>
       </c>
-      <c r="I12" s="12">
+      <c r="K12" s="12">
         <v>1.48</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>18</v>
       </c>
       <c r="B13" s="10">
         <v>65</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="8">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="E13" s="11">
         <v>16</v>
       </c>
-      <c r="D13" s="12">
-        <v>0</v>
-      </c>
-      <c r="E13" s="12">
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="17">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="F13" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="12">
+      <c r="H13" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="12">
         <v>45.5</v>
       </c>
-      <c r="H13" s="12">
+      <c r="J13" s="12">
         <v>2.2200000000000002</v>
       </c>
-      <c r="I13" s="12">
+      <c r="K13" s="12">
         <v>1.68</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>66</v>
       </c>
       <c r="B14" s="10">
         <v>70</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="8">
+        <v>1</v>
+      </c>
+      <c r="D14" s="8">
+        <v>300000</v>
+      </c>
+      <c r="E14" s="11">
         <v>3</v>
       </c>
-      <c r="D14" s="12">
-        <v>0</v>
-      </c>
-      <c r="E14" s="12">
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="F14" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="12">
+      <c r="H14" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
         <v>10</v>
       </c>
-      <c r="H14" s="12">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>66</v>
       </c>
       <c r="B15" s="10">
         <v>70</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="12">
+        <v>300001</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2000000</v>
+      </c>
+      <c r="E15" s="11">
         <v>4</v>
       </c>
-      <c r="D15" s="12">
-        <v>0</v>
-      </c>
-      <c r="E15" s="12">
+      <c r="F15" s="12">
+        <v>0</v>
+      </c>
+      <c r="G15" s="17">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F15" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="12">
+      <c r="H15" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="12">
         <v>10</v>
       </c>
-      <c r="H15" s="12">
-        <v>0</v>
-      </c>
-      <c r="I15" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="12">
+        <v>0</v>
+      </c>
+      <c r="K15" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>71</v>
       </c>
       <c r="B16" s="10">
         <v>75</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8">
+        <v>300000</v>
+      </c>
+      <c r="E16" s="11">
         <v>4</v>
       </c>
-      <c r="D16" s="12">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+      <c r="G16" s="17">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F16" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="12">
+      <c r="H16" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="12">
         <v>10</v>
       </c>
-      <c r="H16" s="12">
-        <v>0</v>
-      </c>
-      <c r="I16" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="12">
+        <v>0</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>71</v>
       </c>
       <c r="B17" s="10">
         <v>75</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="12">
+        <v>300001</v>
+      </c>
+      <c r="D17" s="12">
+        <v>2000000</v>
+      </c>
+      <c r="E17" s="11">
         <v>5</v>
       </c>
-      <c r="D17" s="12">
-        <v>0</v>
-      </c>
-      <c r="E17" s="12">
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
+      <c r="G17" s="17">
         <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="F17" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="12">
+      <c r="H17" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
         <v>10</v>
       </c>
-      <c r="H17" s="12">
-        <v>0</v>
-      </c>
-      <c r="I17" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="12">
+        <v>0</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>76</v>
       </c>
       <c r="B18" s="10">
         <v>80</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8">
+        <v>300000</v>
+      </c>
+      <c r="E18" s="11">
         <v>5</v>
       </c>
-      <c r="D18" s="12">
-        <v>0</v>
-      </c>
-      <c r="E18" s="12">
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+      <c r="G18" s="17">
         <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="F18" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="12">
+      <c r="H18" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="12">
         <v>10</v>
       </c>
-      <c r="H18" s="12">
-        <v>0</v>
-      </c>
-      <c r="I18" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>76</v>
       </c>
       <c r="B19" s="10">
         <v>80</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="12">
+        <v>300001</v>
+      </c>
+      <c r="D19" s="12">
+        <v>2000000</v>
+      </c>
+      <c r="E19" s="11">
         <v>8.75</v>
       </c>
-      <c r="D19" s="12">
-        <v>0</v>
-      </c>
-      <c r="E19" s="12">
+      <c r="F19" s="12">
+        <v>0</v>
+      </c>
+      <c r="G19" s="17">
         <f t="shared" si="0"/>
         <v>0.72916666666666663</v>
       </c>
-      <c r="F19" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="12">
+      <c r="H19" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="12">
         <v>10</v>
       </c>
-      <c r="H19" s="12">
-        <v>0</v>
-      </c>
-      <c r="I19" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="12">
+        <v>0</v>
+      </c>
+      <c r="K19" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>81</v>
       </c>
       <c r="B20" s="14">
         <v>85</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="8">
+        <v>300000</v>
+      </c>
+      <c r="E20" s="11">
         <v>8.75</v>
       </c>
-      <c r="D20" s="12">
-        <v>0</v>
-      </c>
-      <c r="E20" s="12">
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="17">
         <f t="shared" si="0"/>
         <v>0.72916666666666663</v>
       </c>
-      <c r="F20" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="12">
+      <c r="H20" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="12">
         <v>10</v>
       </c>
-      <c r="H20" s="12">
-        <v>0</v>
-      </c>
-      <c r="I20" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15">
-        <v>81</v>
-      </c>
-      <c r="B21" s="16">
-        <v>85</v>
-      </c>
-      <c r="C21" s="17">
-        <v>0</v>
-      </c>
-      <c r="D21" s="12">
-        <v>0</v>
-      </c>
-      <c r="E21" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="12">
-        <v>10</v>
-      </c>
-      <c r="H21" s="18">
-        <v>0</v>
-      </c>
-      <c r="I21" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25">
+        <v>13.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>